<commit_message>
Written some text in report Minor changes
</commit_message>
<xml_diff>
--- a/lab08/references/T2.xlsx
+++ b/lab08/references/T2.xlsx
@@ -107,7 +107,7 @@
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
     <numFmt numFmtId="168" formatCode="0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -139,16 +139,6 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -292,7 +282,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -682,11 +672,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="76183611"/>
-        <c:axId val="31368859"/>
+        <c:axId val="47134656"/>
+        <c:axId val="1681735"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76183611"/>
+        <c:axId val="47134656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,12 +758,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31368859"/>
+        <c:crossAx val="1681735"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31368859"/>
+        <c:axId val="1681735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +845,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76183611"/>
+        <c:crossAx val="47134656"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -882,7 +872,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1236,11 +1226,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="65060797"/>
-        <c:axId val="7674676"/>
+        <c:axId val="2168748"/>
+        <c:axId val="88735142"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65060797"/>
+        <c:axId val="2168748"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,12 +1312,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7674676"/>
+        <c:crossAx val="88735142"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="7674676"/>
+        <c:axId val="88735142"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1409,7 +1399,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65060797"/>
+        <c:crossAx val="2168748"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1436,7 +1426,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1572,11 +1562,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="79975264"/>
-        <c:axId val="23645179"/>
+        <c:axId val="48277680"/>
+        <c:axId val="60359910"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79975264"/>
+        <c:axId val="48277680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,12 +1648,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23645179"/>
+        <c:crossAx val="60359910"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="23645179"/>
+        <c:axId val="60359910"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1745,7 +1735,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79975264"/>
+        <c:crossAx val="48277680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1772,7 +1762,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1802,6 +1792,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2125,11 +2116,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="5631990"/>
-        <c:axId val="22172438"/>
+        <c:axId val="13485343"/>
+        <c:axId val="31035203"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5631990"/>
+        <c:axId val="13485343"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2211,12 +2202,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22172438"/>
+        <c:crossAx val="31035203"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="22172438"/>
+        <c:axId val="31035203"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2298,7 +2289,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5631990"/>
+        <c:crossAx val="13485343"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2325,7 +2316,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2357,12 +2348,14 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="12"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
             </c:dLbl>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2686,11 +2679,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="87161740"/>
-        <c:axId val="51114838"/>
+        <c:axId val="70792749"/>
+        <c:axId val="56342218"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87161740"/>
+        <c:axId val="70792749"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2772,12 +2765,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51114838"/>
+        <c:crossAx val="56342218"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51114838"/>
+        <c:axId val="56342218"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2830,7 +2823,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2859,7 +2852,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87161740"/>
+        <c:crossAx val="70792749"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2886,7 +2879,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2916,6 +2909,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3021,11 +3015,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="37113504"/>
-        <c:axId val="82980136"/>
+        <c:axId val="70067481"/>
+        <c:axId val="8162955"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37113504"/>
+        <c:axId val="70067481"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3078,7 +3072,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3107,12 +3101,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82980136"/>
+        <c:crossAx val="8162955"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82980136"/>
+        <c:axId val="8162955"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3165,7 +3159,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3194,7 +3188,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37113504"/>
+        <c:crossAx val="70067481"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3232,9 +3226,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>835920</xdr:colOff>
+      <xdr:colOff>835560</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3243,7 +3237,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11459520" y="8552160"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3262,9 +3256,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>835920</xdr:colOff>
+      <xdr:colOff>835560</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3273,7 +3267,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11459520" y="12160440"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3292,9 +3286,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>835920</xdr:colOff>
+      <xdr:colOff>835560</xdr:colOff>
       <xdr:row>104</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3303,7 +3297,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11459520" y="15765840"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3322,9 +3316,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>399240</xdr:colOff>
+      <xdr:colOff>398880</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3333,7 +3327,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="798120" y="5308200"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3352,9 +3346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>374760</xdr:colOff>
+      <xdr:colOff>374400</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:rowOff>65880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3363,7 +3357,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="773640" y="8911800"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3382,9 +3376,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>399240</xdr:colOff>
+      <xdr:colOff>398880</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3393,7 +3387,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="798120" y="12771720"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3413,8 +3407,8 @@
   </sheetPr>
   <dimension ref="A1:U114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I90" activeCellId="0" sqref="I90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I42" activeCellId="0" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>